<commit_message>
Add time delay data; update experiment description .xlsx
</commit_message>
<xml_diff>
--- a/experimental_data/data_id_table_031125.xlsx
+++ b/experimental_data/data_id_table_031125.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lut-my.sharepoint.com/personal/mika_virolainen_student_lut_fi/Documents/LUT/6__Research/6_Experimental_Results/measurements_031125/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{33476952-15C5-4EC8-8084-FED8C803CDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59C4BDAC-C32A-4017-8428-89C26C58A36A}"/>
+  <xr:revisionPtr revIDLastSave="440" documentId="8_{33476952-15C5-4EC8-8084-FED8C803CDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DD18AEC-8619-4730-91EF-DB6A3FD9A3AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BF9E0C63-0CF9-442A-A42C-80D3C5BF809C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BF9E0C63-0CF9-442A-A42C-80D3C5BF809C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
   <si>
     <t>CH1 (trigger, coil 1 voltage)</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>again good velocity profile with faster actuation; at the beginning the rack is finding its place (before the test, rack was pushed back and thus synchronization was lost, same situation as in the previous experiments of multiple cycles); 4K 60fps video recorded</t>
+  </si>
+  <si>
+    <t>15.4 µs</t>
+  </si>
+  <si>
+    <t>16.1 µs</t>
   </si>
 </sst>
 </file>
@@ -689,25 +695,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6425C20D-9D0A-445F-83C2-ECBD1706FA63}">
   <dimension ref="D2:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.7109375" style="1"/>
-    <col min="5" max="5" width="75.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="75.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.81640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -733,7 +739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="4:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="4">
         <v>1</v>
       </c>
@@ -755,9 +761,11 @@
       <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D4" s="4">
         <v>2</v>
       </c>
@@ -779,9 +787,11 @@
       <c r="J4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K4" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D5" s="4">
         <v>3</v>
       </c>
@@ -803,9 +813,11 @@
       <c r="J5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D6" s="4">
         <v>4</v>
       </c>
@@ -827,9 +839,11 @@
       <c r="J6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D7" s="4">
         <v>5</v>
       </c>
@@ -851,9 +865,11 @@
       <c r="J7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D8" s="4">
         <v>6</v>
       </c>
@@ -875,9 +891,11 @@
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D9" s="4">
         <v>7</v>
       </c>
@@ -899,9 +917,11 @@
       <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="12" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D12" s="8" t="s">
         <v>3</v>
       </c>
@@ -927,7 +947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D13" s="6">
         <v>8</v>
       </c>
@@ -949,9 +969,11 @@
       <c r="J13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D14" s="6">
         <v>9</v>
       </c>
@@ -973,9 +995,11 @@
       <c r="J14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D15" s="6">
         <v>10</v>
       </c>
@@ -997,9 +1021,11 @@
       <c r="J15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D16" s="6">
         <v>11</v>
       </c>
@@ -1021,9 +1047,11 @@
       <c r="J16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D17" s="6">
         <v>12</v>
       </c>
@@ -1045,17 +1073,19 @@
       <c r="J17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.35">
       <c r="E18" s="10"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
       <c r="E19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D20" s="15" t="s">
         <v>3</v>
       </c>
@@ -1081,7 +1111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="4:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:11" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D21" s="11">
         <v>13</v>
       </c>
@@ -1103,9 +1133,11 @@
       <c r="J21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="11"/>
-    </row>
-    <row r="22" spans="4:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D22" s="13">
         <v>14</v>
       </c>
@@ -1127,9 +1159,11 @@
       <c r="J22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" spans="4:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D23" s="13">
         <v>15</v>
       </c>
@@ -1151,9 +1185,11 @@
       <c r="J23" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="4:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D24" s="13">
         <v>16</v>
       </c>
@@ -1175,9 +1211,11 @@
       <c r="J24" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K24" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D25" s="13">
         <v>17</v>
       </c>
@@ -1199,9 +1237,11 @@
       <c r="J25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="13"/>
-    </row>
-    <row r="26" spans="4:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="K25" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" ht="87" x14ac:dyDescent="0.35">
       <c r="D26" s="13">
         <v>18</v>
       </c>
@@ -1223,9 +1263,11 @@
       <c r="J26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K26" s="13"/>
-    </row>
-    <row r="30" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K26" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D30" s="19" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1293,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="4:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D31" s="17">
         <v>19</v>
       </c>
@@ -1273,9 +1315,11 @@
       <c r="J31" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K31" s="17"/>
-    </row>
-    <row r="32" spans="4:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D32" s="17">
         <v>20</v>
       </c>
@@ -1297,9 +1341,11 @@
       <c r="J32" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K32" s="17"/>
-    </row>
-    <row r="33" spans="4:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D33" s="17">
         <v>21</v>
       </c>
@@ -1319,9 +1365,11 @@
         <v>21</v>
       </c>
       <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-    </row>
-    <row r="34" spans="4:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D34" s="17">
         <v>22</v>
       </c>
@@ -1343,9 +1391,11 @@
       <c r="J34" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K34" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D35" s="17">
         <v>23</v>
       </c>
@@ -1367,9 +1417,11 @@
       <c r="J35" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="17"/>
-    </row>
-    <row r="36" spans="4:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="K35" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" ht="127" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D36" s="17">
         <v>24</v>
       </c>
@@ -1391,10 +1443,13 @@
       <c r="J36" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K36" s="17"/>
+      <c r="K36" s="17" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>